<commit_message>
GB2312 special handling for 0xB0-B2
</commit_message>
<xml_diff>
--- a/Eterm通讯协议.xlsx
+++ b/Eterm通讯协议.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12915" windowHeight="5805" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="12915" windowHeight="5805" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="登陆ETerm通讯" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="198">
   <si>
     <t>f</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -748,10 +748,6 @@
   </si>
   <si>
     <t>超</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不符合规则</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2209,56 +2205,56 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2343,7 +2339,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -16534,8 +16530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="A18:H30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16549,18 +16545,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="C1" s="197" t="s">
+      <c r="C1" s="213" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="197"/>
-      <c r="E1" s="197" t="s">
+      <c r="D1" s="213"/>
+      <c r="E1" s="213" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="197"/>
-      <c r="G1" s="197" t="s">
+      <c r="F1" s="213"/>
+      <c r="G1" s="213" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="197"/>
+      <c r="H1" s="213"/>
     </row>
     <row r="2" spans="1:23" s="104" customFormat="1" ht="16.5">
       <c r="A2" s="112" t="s">
@@ -16592,10 +16588,14 @@
         <v>11010111</v>
       </c>
       <c r="I2" s="115"/>
-      <c r="J2" s="107" t="s">
-        <v>161</v>
-      </c>
-      <c r="K2" s="105"/>
+      <c r="J2" s="107">
+        <f>E2-E3</f>
+        <v>142</v>
+      </c>
+      <c r="K2" s="107">
+        <f>F2-F3</f>
+        <v>128</v>
+      </c>
       <c r="L2" s="105"/>
       <c r="M2" s="105"/>
       <c r="N2" s="105"/>
@@ -16682,8 +16682,14 @@
         <v>10101000</v>
       </c>
       <c r="I4" s="119"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
+      <c r="J4" s="107">
+        <f t="shared" ref="J4:J15" si="2">E4-E5</f>
+        <v>142</v>
+      </c>
+      <c r="K4" s="107">
+        <f t="shared" ref="K4:K15" si="3">F4-F5</f>
+        <v>128</v>
+      </c>
       <c r="L4" s="105"/>
       <c r="M4" s="105"/>
       <c r="N4" s="105"/>
@@ -16709,19 +16715,19 @@
         <v>28</v>
       </c>
       <c r="E5" s="117">
-        <f t="shared" ref="E5:E15" si="2">HEX2DEC(C5)</f>
+        <f t="shared" ref="E5:E15" si="4">HEX2DEC(C5)</f>
         <v>35</v>
       </c>
       <c r="F5" s="117">
-        <f t="shared" ref="F5:F15" si="3">HEX2DEC(D5)</f>
+        <f t="shared" ref="F5:F15" si="5">HEX2DEC(D5)</f>
         <v>40</v>
       </c>
       <c r="G5" s="118" t="str">
-        <f t="shared" ref="G5:G15" si="4">DEC2BIN(E5,8)</f>
+        <f t="shared" ref="G5:G15" si="6">DEC2BIN(E5,8)</f>
         <v>00100011</v>
       </c>
       <c r="H5" s="118" t="str">
-        <f t="shared" ref="H5:H15" si="5">DEC2BIN(F5,8)</f>
+        <f t="shared" ref="H5:H15" si="7">DEC2BIN(F5,8)</f>
         <v>00101000</v>
       </c>
       <c r="I5" s="119"/>
@@ -16754,24 +16760,30 @@
         <v>144</v>
       </c>
       <c r="E6" s="117">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>178</v>
       </c>
       <c r="F6" s="117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>204</v>
       </c>
       <c r="G6" s="118" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10110010</v>
       </c>
       <c r="H6" s="118" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11001100</v>
       </c>
       <c r="I6" s="119"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
+      <c r="J6" s="107">
+        <f t="shared" ref="J6:J15" si="8">E6-E7</f>
+        <v>142</v>
+      </c>
+      <c r="K6" s="107">
+        <f t="shared" ref="K6:K15" si="9">F6-F7</f>
+        <v>128</v>
+      </c>
       <c r="L6" s="105"/>
       <c r="M6" s="105"/>
       <c r="N6" s="105"/>
@@ -16797,19 +16809,19 @@
         <v>145</v>
       </c>
       <c r="E7" s="121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="F7" s="121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>76</v>
       </c>
       <c r="G7" s="122" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>00100100</v>
       </c>
       <c r="H7" s="122" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>01001100</v>
       </c>
       <c r="I7" s="123"/>
@@ -16842,24 +16854,30 @@
         <v>159</v>
       </c>
       <c r="E8" s="105">
-        <f t="shared" ref="E8:E9" si="6">HEX2DEC(C8)</f>
+        <f t="shared" ref="E8:E9" si="10">HEX2DEC(C8)</f>
         <v>179</v>
       </c>
       <c r="F8" s="105">
-        <f t="shared" ref="F8:F9" si="7">HEX2DEC(D8)</f>
+        <f t="shared" ref="F8:F9" si="11">HEX2DEC(D8)</f>
         <v>172</v>
       </c>
       <c r="G8" s="111" t="str">
-        <f t="shared" ref="G8:G9" si="8">DEC2BIN(E8,8)</f>
+        <f t="shared" ref="G8:G9" si="12">DEC2BIN(E8,8)</f>
         <v>10110011</v>
       </c>
       <c r="H8" s="111" t="str">
-        <f t="shared" ref="H8:H9" si="9">DEC2BIN(F8,8)</f>
+        <f t="shared" ref="H8:H9" si="13">DEC2BIN(F8,8)</f>
         <v>10101100</v>
       </c>
       <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
+      <c r="J8" s="107">
+        <f t="shared" ref="J8:J15" si="14">E8-E9</f>
+        <v>128</v>
+      </c>
+      <c r="K8" s="107">
+        <f t="shared" ref="K8:K15" si="15">F8-F9</f>
+        <v>128</v>
+      </c>
       <c r="L8" s="105"/>
       <c r="M8" s="105"/>
       <c r="N8" s="105"/>
@@ -16885,19 +16903,19 @@
         <v>157</v>
       </c>
       <c r="E9" s="105">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>51</v>
       </c>
       <c r="F9" s="105">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>44</v>
       </c>
       <c r="G9" s="111" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>00110011</v>
       </c>
       <c r="H9" s="111" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>00101100</v>
       </c>
       <c r="I9" s="105"/>
@@ -16930,26 +16948,32 @@
         <v>155</v>
       </c>
       <c r="E10" s="105">
-        <f t="shared" ref="E10:F12" si="10">HEX2DEC(C10)</f>
+        <f t="shared" ref="E10:F12" si="16">HEX2DEC(C10)</f>
         <v>180</v>
       </c>
       <c r="F10" s="105">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>207</v>
       </c>
       <c r="G10" s="111" t="str">
-        <f t="shared" ref="G10:H12" si="11">DEC2BIN(E10,8)</f>
+        <f t="shared" ref="G10:H12" si="17">DEC2BIN(E10,8)</f>
         <v>10110100</v>
       </c>
       <c r="H10" s="111" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>11001111</v>
       </c>
       <c r="I10" s="107" t="s">
         <v>149</v>
       </c>
-      <c r="J10" s="105"/>
-      <c r="K10" s="105"/>
+      <c r="J10" s="107">
+        <f t="shared" ref="J10:J15" si="18">E10-E11</f>
+        <v>128</v>
+      </c>
+      <c r="K10" s="107">
+        <f t="shared" ref="K10:K15" si="19">F10-F11</f>
+        <v>128</v>
+      </c>
       <c r="L10" s="105"/>
       <c r="M10" s="105"/>
       <c r="N10" s="105"/>
@@ -16975,19 +16999,19 @@
         <v>153</v>
       </c>
       <c r="E11" s="105">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>52</v>
       </c>
       <c r="F11" s="105">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>79</v>
       </c>
       <c r="G11" s="111" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>00110100</v>
       </c>
       <c r="H11" s="111" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>01001111</v>
       </c>
       <c r="I11" s="105"/>
@@ -17020,26 +17044,32 @@
         <v>152</v>
       </c>
       <c r="E12" s="105">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>181</v>
       </c>
       <c r="F12" s="105">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>164</v>
       </c>
       <c r="G12" s="111" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>10110101</v>
       </c>
       <c r="H12" s="111" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>10100100</v>
       </c>
       <c r="I12" s="107" t="s">
         <v>149</v>
       </c>
-      <c r="J12" s="105"/>
-      <c r="K12" s="105"/>
+      <c r="J12" s="107">
+        <f t="shared" ref="J12:J15" si="20">E12-E13</f>
+        <v>128</v>
+      </c>
+      <c r="K12" s="107">
+        <f t="shared" ref="K12:K15" si="21">F12-F13</f>
+        <v>128</v>
+      </c>
       <c r="L12" s="105"/>
       <c r="M12" s="105"/>
       <c r="N12" s="105"/>
@@ -17065,19 +17095,19 @@
         <v>24</v>
       </c>
       <c r="E13" s="105">
-        <f t="shared" ref="E13" si="12">HEX2DEC(C13)</f>
+        <f t="shared" ref="E13" si="22">HEX2DEC(C13)</f>
         <v>53</v>
       </c>
       <c r="F13" s="105">
-        <f t="shared" ref="F13" si="13">HEX2DEC(D13)</f>
+        <f t="shared" ref="F13" si="23">HEX2DEC(D13)</f>
         <v>36</v>
       </c>
       <c r="G13" s="111" t="str">
-        <f t="shared" ref="G13" si="14">DEC2BIN(E13,8)</f>
+        <f t="shared" ref="G13" si="24">DEC2BIN(E13,8)</f>
         <v>00110101</v>
       </c>
       <c r="H13" s="111" t="str">
-        <f t="shared" ref="H13" si="15">DEC2BIN(F13,8)</f>
+        <f t="shared" ref="H13" si="25">DEC2BIN(F13,8)</f>
         <v>00100100</v>
       </c>
       <c r="I13" s="105"/>
@@ -17110,26 +17140,32 @@
         <v>148</v>
       </c>
       <c r="E14" s="105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>182</v>
       </c>
       <c r="F14" s="105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>161</v>
       </c>
       <c r="G14" s="111" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10110110</v>
       </c>
       <c r="H14" s="111" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10100001</v>
       </c>
       <c r="I14" s="107" t="s">
         <v>149</v>
       </c>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
+      <c r="J14" s="107">
+        <f t="shared" ref="J14:J15" si="26">E14-E15</f>
+        <v>128</v>
+      </c>
+      <c r="K14" s="107">
+        <f t="shared" ref="K14:K15" si="27">F14-F15</f>
+        <v>128</v>
+      </c>
       <c r="L14" s="105"/>
       <c r="M14" s="105"/>
       <c r="N14" s="105"/>
@@ -17155,19 +17191,19 @@
         <v>21</v>
       </c>
       <c r="E15" s="105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="F15" s="105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="G15" s="111" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>00110110</v>
       </c>
       <c r="H15" s="111" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>00100001</v>
       </c>
       <c r="I15" s="105"/>
@@ -17285,8 +17321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -17304,13 +17340,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.5">
       <c r="A1" s="110" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="124" t="s">
         <v>162</v>
-      </c>
-      <c r="C1" s="124" t="s">
-        <v>163</v>
       </c>
       <c r="D1" s="125"/>
       <c r="E1" s="125">
@@ -17347,7 +17383,7 @@
         <v>78</v>
       </c>
       <c r="D2" s="118" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E2" s="118">
         <v>64</v>
@@ -17398,13 +17434,13 @@
     </row>
     <row r="3" spans="1:17" ht="14.25">
       <c r="A3" s="140" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="141" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="141" t="s">
+      <c r="C3" s="148" t="s">
         <v>167</v>
-      </c>
-      <c r="C3" s="148" t="s">
-        <v>168</v>
       </c>
       <c r="D3" s="142"/>
       <c r="E3" s="142">
@@ -17492,10 +17528,10 @@
     </row>
     <row r="5" spans="1:17" ht="14.25">
       <c r="A5" s="109" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C5" s="148">
         <v>90</v>
@@ -17525,7 +17561,7 @@
         <v>01000010</v>
       </c>
       <c r="Q5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" thickBot="1">
@@ -17586,22 +17622,22 @@
         <v>1</v>
       </c>
       <c r="Q6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="14.25">
       <c r="A7" s="140" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="157" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="148" t="s">
         <v>170</v>
-      </c>
-      <c r="B7" s="157" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="148" t="s">
-        <v>171</v>
       </c>
       <c r="D7" s="142"/>
       <c r="E7" s="142" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" s="149"/>
       <c r="G7" s="152">
@@ -17625,7 +17661,7 @@
       </c>
       <c r="N7" s="137"/>
       <c r="Q7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15" thickBot="1">
@@ -17686,22 +17722,22 @@
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="14.25">
       <c r="A9" s="140" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" s="157" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="148" t="s">
         <v>173</v>
-      </c>
-      <c r="B9" s="157" t="s">
-        <v>167</v>
-      </c>
-      <c r="C9" s="148" t="s">
-        <v>174</v>
       </c>
       <c r="D9" s="142"/>
       <c r="E9" s="142" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F9" s="149"/>
       <c r="G9" s="152">
@@ -17785,17 +17821,17 @@
     </row>
     <row r="11" spans="1:17" ht="14.25">
       <c r="A11" s="140" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="157" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="148" t="s">
         <v>175</v>
-      </c>
-      <c r="B11" s="157" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="148" t="s">
-        <v>176</v>
       </c>
       <c r="D11" s="142"/>
       <c r="E11" s="142" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F11" s="149"/>
       <c r="G11" s="152">
@@ -17879,17 +17915,17 @@
     </row>
     <row r="13" spans="1:17" ht="14.25">
       <c r="A13" s="140" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B13" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C13" s="148" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D13" s="142"/>
       <c r="E13" s="142" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F13" s="149"/>
       <c r="G13" s="152">
@@ -17973,13 +18009,13 @@
     </row>
     <row r="15" spans="1:17" ht="14.25">
       <c r="A15" s="140" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" s="148" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D15" s="142"/>
       <c r="E15" s="142">
@@ -18067,13 +18103,13 @@
     </row>
     <row r="17" spans="1:16" ht="14.25">
       <c r="A17" s="140" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B17" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" s="148" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D17" s="142"/>
       <c r="E17" s="142">
@@ -18162,7 +18198,7 @@
     <row r="19" spans="1:16" ht="14.25">
       <c r="A19" s="140"/>
       <c r="B19" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" s="148">
         <v>81</v>
@@ -18256,14 +18292,14 @@
     <row r="21" spans="1:16" ht="14.25">
       <c r="A21" s="140"/>
       <c r="B21" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C21" s="148">
         <v>81</v>
       </c>
       <c r="D21" s="142"/>
       <c r="E21" s="142" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F21" s="149"/>
       <c r="G21" s="152">
@@ -18348,7 +18384,7 @@
     <row r="23" spans="1:16" ht="14.25">
       <c r="A23" s="140"/>
       <c r="B23" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="148">
         <v>81</v>
@@ -18440,7 +18476,7 @@
     <row r="25" spans="1:16" ht="14.25">
       <c r="A25" s="140"/>
       <c r="B25" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C25" s="148">
         <v>82</v>
@@ -18532,7 +18568,7 @@
     <row r="27" spans="1:16" ht="14.25">
       <c r="A27" s="140"/>
       <c r="B27" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" s="148">
         <v>83</v>
@@ -18624,7 +18660,7 @@
     <row r="29" spans="1:16" ht="14.25">
       <c r="A29" s="140"/>
       <c r="B29" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" s="148">
         <v>84</v>
@@ -18716,7 +18752,7 @@
     <row r="31" spans="1:16" ht="14.25">
       <c r="A31" s="140"/>
       <c r="B31" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C31" s="148">
         <v>85</v>
@@ -18808,7 +18844,7 @@
     <row r="33" spans="1:16" ht="14.25">
       <c r="A33" s="140"/>
       <c r="B33" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C33" s="148"/>
       <c r="D33" s="142"/>
@@ -18888,7 +18924,7 @@
     <row r="35" spans="1:16" ht="14.25">
       <c r="A35" s="140"/>
       <c r="B35" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C35" s="148"/>
       <c r="D35" s="142"/>
@@ -18967,17 +19003,17 @@
     </row>
     <row r="37" spans="1:16" ht="14.25">
       <c r="A37" s="140" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B37" s="157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" s="148" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D37" s="142"/>
       <c r="E37" s="142" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F37" s="149"/>
       <c r="G37" s="152">
@@ -19061,17 +19097,17 @@
     </row>
     <row r="39" spans="1:16" ht="14.25">
       <c r="A39" t="s">
+        <v>190</v>
+      </c>
+      <c r="B39" s="212" t="s">
         <v>191</v>
       </c>
-      <c r="B39" s="213" t="s">
-        <v>192</v>
-      </c>
       <c r="C39" s="148" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D39" s="142"/>
       <c r="E39" s="142" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F39" s="149"/>
       <c r="G39" s="152">
@@ -19096,8 +19132,8 @@
       <c r="N39" s="137"/>
     </row>
     <row r="40" spans="1:16" ht="15" thickBot="1">
-      <c r="B40" s="213" t="s">
-        <v>193</v>
+      <c r="B40" s="212" t="s">
+        <v>192</v>
       </c>
       <c r="C40" s="150" t="str">
         <f t="shared" ref="C40" si="178">DEC2HEX(G40)</f>
@@ -19163,8 +19199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -19222,75 +19258,75 @@
       <c r="X1" s="183"/>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="212"/>
-      <c r="B2" s="200"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="201"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="203" t="str">
+      <c r="A2" s="211"/>
+      <c r="B2" s="199"/>
+      <c r="C2" s="199"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="199"/>
+      <c r="F2" s="199"/>
+      <c r="G2" s="199"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="202" t="str">
         <f>MID(TEXT(HEX2BIN($I1,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="J2" s="204" t="str">
+      <c r="J2" s="203" t="str">
         <f>MID(TEXT(HEX2BIN($I1,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="204" t="str">
+      <c r="K2" s="203" t="str">
         <f>MID(TEXT(HEX2BIN($I1,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="L2" s="204" t="str">
+      <c r="L2" s="203" t="str">
         <f>MID(TEXT(HEX2BIN($I1,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="205" t="str">
+      <c r="M2" s="204" t="str">
         <f>MID(TEXT(HEX2BIN($M1,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="N2" s="206" t="str">
+      <c r="N2" s="205" t="str">
         <f>MID(TEXT(HEX2BIN($M1,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="O2" s="206" t="str">
+      <c r="O2" s="205" t="str">
         <f>MID(TEXT(HEX2BIN($M1,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="P2" s="207" t="str">
+      <c r="P2" s="206" t="str">
         <f>MID(TEXT(HEX2BIN($M1,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
-      <c r="Q2" s="208" t="str">
+      <c r="Q2" s="207" t="str">
         <f>MID(TEXT(HEX2BIN($Q1,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="R2" s="209" t="str">
+      <c r="R2" s="208" t="str">
         <f>MID(TEXT(HEX2BIN($Q1,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="S2" s="209" t="str">
+      <c r="S2" s="208" t="str">
         <f>MID(TEXT(HEX2BIN($Q1,4),"0000"),3,1)</f>
         <v>1</v>
       </c>
-      <c r="T2" s="209" t="str">
+      <c r="T2" s="208" t="str">
         <f>MID(TEXT(HEX2BIN($Q1,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
-      <c r="U2" s="210" t="str">
+      <c r="U2" s="209" t="str">
         <f>MID(TEXT(HEX2BIN($U1,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="V2" s="209" t="str">
+      <c r="V2" s="208" t="str">
         <f>MID(TEXT(HEX2BIN($U1,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="W2" s="209" t="str">
+      <c r="W2" s="208" t="str">
         <f>MID(TEXT(HEX2BIN($U1,4),"0000"),3,1)</f>
         <v>1</v>
       </c>
-      <c r="X2" s="211" t="str">
+      <c r="X2" s="210" t="str">
         <f>MID(TEXT(HEX2BIN($U1,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
@@ -19350,19 +19386,19 @@
         <f>MID(TEXT(HEX2BIN($A3,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="198" t="str">
+      <c r="E4" s="197" t="str">
         <f>MID(TEXT(HEX2BIN($E3,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="F4" s="198" t="str">
+      <c r="F4" s="197" t="str">
         <f>MID(TEXT(HEX2BIN($E3,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="198" t="str">
+      <c r="G4" s="197" t="str">
         <f>MID(TEXT(HEX2BIN($E3,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="199" t="str">
+      <c r="H4" s="198" t="str">
         <f>MID(TEXT(HEX2BIN($E3,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
@@ -19466,75 +19502,75 @@
       <c r="X5" s="183"/>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="212"/>
-      <c r="B6" s="200"/>
-      <c r="C6" s="200"/>
-      <c r="D6" s="201"/>
-      <c r="E6" s="200"/>
-      <c r="F6" s="200"/>
-      <c r="G6" s="200"/>
-      <c r="H6" s="202"/>
-      <c r="I6" s="203" t="str">
+      <c r="A6" s="211"/>
+      <c r="B6" s="199"/>
+      <c r="C6" s="199"/>
+      <c r="D6" s="200"/>
+      <c r="E6" s="199"/>
+      <c r="F6" s="199"/>
+      <c r="G6" s="199"/>
+      <c r="H6" s="201"/>
+      <c r="I6" s="202" t="str">
         <f>MID(TEXT(HEX2BIN($I5,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="J6" s="204" t="str">
+      <c r="J6" s="203" t="str">
         <f>MID(TEXT(HEX2BIN($I5,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="204" t="str">
+      <c r="K6" s="203" t="str">
         <f>MID(TEXT(HEX2BIN($I5,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="204" t="str">
+      <c r="L6" s="203" t="str">
         <f>MID(TEXT(HEX2BIN($I5,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="205" t="str">
+      <c r="M6" s="204" t="str">
         <f>MID(TEXT(HEX2BIN($M5,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="206" t="str">
+      <c r="N6" s="205" t="str">
         <f>MID(TEXT(HEX2BIN($M5,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="O6" s="206" t="str">
+      <c r="O6" s="205" t="str">
         <f>MID(TEXT(HEX2BIN($M5,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="P6" s="207" t="str">
+      <c r="P6" s="206" t="str">
         <f>MID(TEXT(HEX2BIN($M5,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
-      <c r="Q6" s="208" t="str">
+      <c r="Q6" s="207" t="str">
         <f>MID(TEXT(HEX2BIN($Q5,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="R6" s="209" t="str">
+      <c r="R6" s="208" t="str">
         <f>MID(TEXT(HEX2BIN($Q5,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="S6" s="209" t="str">
+      <c r="S6" s="208" t="str">
         <f>MID(TEXT(HEX2BIN($Q5,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="T6" s="209" t="str">
+      <c r="T6" s="208" t="str">
         <f>MID(TEXT(HEX2BIN($Q5,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="U6" s="210" t="str">
+      <c r="U6" s="209" t="str">
         <f>MID(TEXT(HEX2BIN($U5,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="V6" s="209" t="str">
+      <c r="V6" s="208" t="str">
         <f>MID(TEXT(HEX2BIN($U5,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="W6" s="209" t="str">
+      <c r="W6" s="208" t="str">
         <f>MID(TEXT(HEX2BIN($U5,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="X6" s="211" t="str">
+      <c r="X6" s="210" t="str">
         <f>MID(TEXT(HEX2BIN($U5,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
@@ -19594,19 +19630,19 @@
         <f>MID(TEXT(HEX2BIN($A7,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="198" t="str">
+      <c r="E8" s="197" t="str">
         <f>MID(TEXT(HEX2BIN($E7,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="198" t="str">
+      <c r="F8" s="197" t="str">
         <f>MID(TEXT(HEX2BIN($E7,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="G8" s="198" t="str">
+      <c r="G8" s="197" t="str">
         <f>MID(TEXT(HEX2BIN($E7,4),"0000"),3,1)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="199" t="str">
+      <c r="H8" s="198" t="str">
         <f>MID(TEXT(HEX2BIN($E7,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
@@ -19710,75 +19746,75 @@
       <c r="X9" s="183"/>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="212"/>
-      <c r="B10" s="200"/>
-      <c r="C10" s="200"/>
-      <c r="D10" s="201"/>
-      <c r="E10" s="200"/>
-      <c r="F10" s="200"/>
-      <c r="G10" s="200"/>
-      <c r="H10" s="202"/>
-      <c r="I10" s="203" t="str">
+      <c r="A10" s="211"/>
+      <c r="B10" s="199"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="200"/>
+      <c r="E10" s="199"/>
+      <c r="F10" s="199"/>
+      <c r="G10" s="199"/>
+      <c r="H10" s="201"/>
+      <c r="I10" s="202" t="str">
         <f t="shared" ref="I10" si="0">MID(TEXT(HEX2BIN($I9,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="J10" s="204" t="str">
+      <c r="J10" s="203" t="str">
         <f t="shared" ref="J10" si="1">MID(TEXT(HEX2BIN($I9,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="204" t="str">
+      <c r="K10" s="203" t="str">
         <f t="shared" ref="K10" si="2">MID(TEXT(HEX2BIN($I9,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="L10" s="204" t="str">
+      <c r="L10" s="203" t="str">
         <f t="shared" ref="L10" si="3">MID(TEXT(HEX2BIN($I9,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="M10" s="205" t="str">
+      <c r="M10" s="204" t="str">
         <f t="shared" ref="M10" si="4">MID(TEXT(HEX2BIN($M9,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="N10" s="206" t="str">
+      <c r="N10" s="205" t="str">
         <f t="shared" ref="N10" si="5">MID(TEXT(HEX2BIN($M9,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="O10" s="206" t="str">
+      <c r="O10" s="205" t="str">
         <f t="shared" ref="O10" si="6">MID(TEXT(HEX2BIN($M9,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="P10" s="207" t="str">
+      <c r="P10" s="206" t="str">
         <f t="shared" ref="P10" si="7">MID(TEXT(HEX2BIN($M9,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="208" t="str">
+      <c r="Q10" s="207" t="str">
         <f t="shared" ref="Q10" si="8">MID(TEXT(HEX2BIN($Q9,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="R10" s="209" t="str">
+      <c r="R10" s="208" t="str">
         <f t="shared" ref="R10" si="9">MID(TEXT(HEX2BIN($Q9,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="S10" s="209" t="str">
+      <c r="S10" s="208" t="str">
         <f t="shared" ref="S10" si="10">MID(TEXT(HEX2BIN($Q9,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="T10" s="209" t="str">
+      <c r="T10" s="208" t="str">
         <f t="shared" ref="T10" si="11">MID(TEXT(HEX2BIN($Q9,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="U10" s="210" t="str">
+      <c r="U10" s="209" t="str">
         <f t="shared" ref="U10" si="12">MID(TEXT(HEX2BIN($U9,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="V10" s="209" t="str">
+      <c r="V10" s="208" t="str">
         <f t="shared" ref="V10" si="13">MID(TEXT(HEX2BIN($U9,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="W10" s="209" t="str">
+      <c r="W10" s="208" t="str">
         <f t="shared" ref="W10" si="14">MID(TEXT(HEX2BIN($U9,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="X10" s="211" t="str">
+      <c r="X10" s="210" t="str">
         <f t="shared" ref="X10" si="15">MID(TEXT(HEX2BIN($U9,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
@@ -19838,19 +19874,19 @@
         <f t="shared" ref="D12" si="19">MID(TEXT(HEX2BIN($A11,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="198" t="str">
+      <c r="E12" s="197" t="str">
         <f t="shared" ref="E12" si="20">MID(TEXT(HEX2BIN($E11,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="198" t="str">
+      <c r="F12" s="197" t="str">
         <f t="shared" ref="F12" si="21">MID(TEXT(HEX2BIN($E11,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="G12" s="198" t="str">
+      <c r="G12" s="197" t="str">
         <f t="shared" ref="G12" si="22">MID(TEXT(HEX2BIN($E11,4),"0000"),3,1)</f>
         <v>1</v>
       </c>
-      <c r="H12" s="199" t="str">
+      <c r="H12" s="198" t="str">
         <f t="shared" ref="H12" si="23">MID(TEXT(HEX2BIN($E11,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
@@ -19935,7 +19971,7 @@
       <c r="K13" s="180"/>
       <c r="L13" s="180"/>
       <c r="M13" s="182" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N13" s="180"/>
       <c r="O13" s="180"/>
@@ -19954,75 +19990,75 @@
       <c r="X13" s="183"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="212"/>
-      <c r="B14" s="200"/>
-      <c r="C14" s="200"/>
-      <c r="D14" s="201"/>
-      <c r="E14" s="200"/>
-      <c r="F14" s="200"/>
-      <c r="G14" s="200"/>
-      <c r="H14" s="202"/>
-      <c r="I14" s="203" t="str">
+      <c r="A14" s="211"/>
+      <c r="B14" s="199"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="200"/>
+      <c r="E14" s="199"/>
+      <c r="F14" s="199"/>
+      <c r="G14" s="199"/>
+      <c r="H14" s="201"/>
+      <c r="I14" s="202" t="str">
         <f t="shared" ref="I14" si="40">MID(TEXT(HEX2BIN($I13,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="J14" s="204" t="str">
+      <c r="J14" s="203" t="str">
         <f t="shared" ref="J14" si="41">MID(TEXT(HEX2BIN($I13,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="204" t="str">
+      <c r="K14" s="203" t="str">
         <f t="shared" ref="K14" si="42">MID(TEXT(HEX2BIN($I13,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="204" t="str">
+      <c r="L14" s="203" t="str">
         <f t="shared" ref="L14" si="43">MID(TEXT(HEX2BIN($I13,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
-      <c r="M14" s="205" t="str">
+      <c r="M14" s="204" t="str">
         <f t="shared" ref="M14" si="44">MID(TEXT(HEX2BIN($M13,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="N14" s="206" t="str">
+      <c r="N14" s="205" t="str">
         <f t="shared" ref="N14" si="45">MID(TEXT(HEX2BIN($M13,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="O14" s="206" t="str">
+      <c r="O14" s="205" t="str">
         <f t="shared" ref="O14" si="46">MID(TEXT(HEX2BIN($M13,4),"0000"),3,1)</f>
         <v>1</v>
       </c>
-      <c r="P14" s="207" t="str">
+      <c r="P14" s="206" t="str">
         <f t="shared" ref="P14" si="47">MID(TEXT(HEX2BIN($M13,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
-      <c r="Q14" s="208" t="str">
+      <c r="Q14" s="207" t="str">
         <f t="shared" ref="Q14" si="48">MID(TEXT(HEX2BIN($Q13,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="R14" s="209" t="str">
+      <c r="R14" s="208" t="str">
         <f t="shared" ref="R14" si="49">MID(TEXT(HEX2BIN($Q13,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="S14" s="209" t="str">
+      <c r="S14" s="208" t="str">
         <f t="shared" ref="S14" si="50">MID(TEXT(HEX2BIN($Q13,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="T14" s="209" t="str">
+      <c r="T14" s="208" t="str">
         <f t="shared" ref="T14" si="51">MID(TEXT(HEX2BIN($Q13,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
-      <c r="U14" s="210" t="str">
+      <c r="U14" s="209" t="str">
         <f t="shared" ref="U14" si="52">MID(TEXT(HEX2BIN($U13,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="209" t="str">
+      <c r="V14" s="208" t="str">
         <f t="shared" ref="V14" si="53">MID(TEXT(HEX2BIN($U13,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="W14" s="209" t="str">
+      <c r="W14" s="208" t="str">
         <f t="shared" ref="W14" si="54">MID(TEXT(HEX2BIN($U13,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="X14" s="211" t="str">
+      <c r="X14" s="210" t="str">
         <f t="shared" ref="X14" si="55">MID(TEXT(HEX2BIN($U13,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
@@ -20082,19 +20118,19 @@
         <f t="shared" ref="D16" si="59">MID(TEXT(HEX2BIN($A15,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="198" t="str">
+      <c r="E16" s="197" t="str">
         <f t="shared" ref="E16" si="60">MID(TEXT(HEX2BIN($E15,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="F16" s="198" t="str">
+      <c r="F16" s="197" t="str">
         <f t="shared" ref="F16" si="61">MID(TEXT(HEX2BIN($E15,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="198" t="str">
+      <c r="G16" s="197" t="str">
         <f t="shared" ref="G16" si="62">MID(TEXT(HEX2BIN($E15,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="199" t="str">
+      <c r="H16" s="198" t="str">
         <f t="shared" ref="H16" si="63">MID(TEXT(HEX2BIN($E15,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
@@ -20173,7 +20209,7 @@
       <c r="G17" s="180"/>
       <c r="H17" s="183"/>
       <c r="I17" s="184" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J17" s="180"/>
       <c r="K17" s="180"/>
@@ -20198,75 +20234,75 @@
       <c r="X17" s="183"/>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="212"/>
-      <c r="B18" s="200"/>
-      <c r="C18" s="200"/>
-      <c r="D18" s="201"/>
-      <c r="E18" s="200"/>
-      <c r="F18" s="200"/>
-      <c r="G18" s="200"/>
-      <c r="H18" s="202"/>
-      <c r="I18" s="203" t="str">
+      <c r="A18" s="211"/>
+      <c r="B18" s="199"/>
+      <c r="C18" s="199"/>
+      <c r="D18" s="200"/>
+      <c r="E18" s="199"/>
+      <c r="F18" s="199"/>
+      <c r="G18" s="199"/>
+      <c r="H18" s="201"/>
+      <c r="I18" s="202" t="str">
         <f t="shared" ref="I18" si="80">MID(TEXT(HEX2BIN($I17,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="J18" s="204" t="str">
+      <c r="J18" s="203" t="str">
         <f t="shared" ref="J18" si="81">MID(TEXT(HEX2BIN($I17,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="K18" s="204" t="str">
+      <c r="K18" s="203" t="str">
         <f t="shared" ref="K18" si="82">MID(TEXT(HEX2BIN($I17,4),"0000"),3,1)</f>
         <v>1</v>
       </c>
-      <c r="L18" s="204" t="str">
+      <c r="L18" s="203" t="str">
         <f t="shared" ref="L18" si="83">MID(TEXT(HEX2BIN($I17,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="M18" s="205" t="str">
+      <c r="M18" s="204" t="str">
         <f t="shared" ref="M18" si="84">MID(TEXT(HEX2BIN($M17,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="N18" s="206" t="str">
+      <c r="N18" s="205" t="str">
         <f t="shared" ref="N18" si="85">MID(TEXT(HEX2BIN($M17,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="O18" s="206" t="str">
+      <c r="O18" s="205" t="str">
         <f t="shared" ref="O18" si="86">MID(TEXT(HEX2BIN($M17,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="P18" s="207" t="str">
+      <c r="P18" s="206" t="str">
         <f t="shared" ref="P18" si="87">MID(TEXT(HEX2BIN($M17,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
-      <c r="Q18" s="208" t="str">
+      <c r="Q18" s="207" t="str">
         <f t="shared" ref="Q18" si="88">MID(TEXT(HEX2BIN($Q17,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="R18" s="209" t="str">
+      <c r="R18" s="208" t="str">
         <f t="shared" ref="R18" si="89">MID(TEXT(HEX2BIN($Q17,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="S18" s="209" t="str">
+      <c r="S18" s="208" t="str">
         <f t="shared" ref="S18" si="90">MID(TEXT(HEX2BIN($Q17,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="T18" s="209" t="str">
+      <c r="T18" s="208" t="str">
         <f t="shared" ref="T18" si="91">MID(TEXT(HEX2BIN($Q17,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="U18" s="210" t="str">
+      <c r="U18" s="209" t="str">
         <f t="shared" ref="U18" si="92">MID(TEXT(HEX2BIN($U17,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="V18" s="209" t="str">
+      <c r="V18" s="208" t="str">
         <f t="shared" ref="V18" si="93">MID(TEXT(HEX2BIN($U17,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="W18" s="209" t="str">
+      <c r="W18" s="208" t="str">
         <f t="shared" ref="W18" si="94">MID(TEXT(HEX2BIN($U17,4),"0000"),3,1)</f>
         <v>1</v>
       </c>
-      <c r="X18" s="211" t="str">
+      <c r="X18" s="210" t="str">
         <f t="shared" ref="X18" si="95">MID(TEXT(HEX2BIN($U17,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
@@ -20279,7 +20315,7 @@
       <c r="C19" s="186"/>
       <c r="D19" s="187"/>
       <c r="E19" s="186" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F19" s="186"/>
       <c r="G19" s="186"/>
@@ -20326,19 +20362,19 @@
         <f t="shared" ref="D20" si="99">MID(TEXT(HEX2BIN($A19,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="198" t="str">
+      <c r="E20" s="197" t="str">
         <f t="shared" ref="E20" si="100">MID(TEXT(HEX2BIN($E19,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="F20" s="198" t="str">
+      <c r="F20" s="197" t="str">
         <f t="shared" ref="F20" si="101">MID(TEXT(HEX2BIN($E19,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="G20" s="198" t="str">
+      <c r="G20" s="197" t="str">
         <f t="shared" ref="G20" si="102">MID(TEXT(HEX2BIN($E19,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="199" t="str">
+      <c r="H20" s="198" t="str">
         <f t="shared" ref="H20" si="103">MID(TEXT(HEX2BIN($E19,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
@@ -20417,19 +20453,19 @@
       <c r="G21" s="180"/>
       <c r="H21" s="183"/>
       <c r="I21" s="184" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J21" s="180"/>
       <c r="K21" s="180"/>
       <c r="L21" s="180"/>
       <c r="M21" s="182" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N21" s="180"/>
       <c r="O21" s="180"/>
       <c r="P21" s="183"/>
       <c r="Q21" s="184" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R21" s="180"/>
       <c r="S21" s="180"/>
@@ -20442,75 +20478,75 @@
       <c r="X21" s="183"/>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="212"/>
-      <c r="B22" s="200"/>
-      <c r="C22" s="200"/>
-      <c r="D22" s="201"/>
-      <c r="E22" s="200"/>
-      <c r="F22" s="200"/>
-      <c r="G22" s="200"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="203" t="str">
+      <c r="A22" s="211"/>
+      <c r="B22" s="199"/>
+      <c r="C22" s="199"/>
+      <c r="D22" s="200"/>
+      <c r="E22" s="199"/>
+      <c r="F22" s="199"/>
+      <c r="G22" s="199"/>
+      <c r="H22" s="201"/>
+      <c r="I22" s="202" t="str">
         <f t="shared" ref="I22" si="120">MID(TEXT(HEX2BIN($I21,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="J22" s="204" t="str">
+      <c r="J22" s="203" t="str">
         <f t="shared" ref="J22" si="121">MID(TEXT(HEX2BIN($I21,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="K22" s="204" t="str">
+      <c r="K22" s="203" t="str">
         <f t="shared" ref="K22" si="122">MID(TEXT(HEX2BIN($I21,4),"0000"),3,1)</f>
         <v>1</v>
       </c>
-      <c r="L22" s="204" t="str">
+      <c r="L22" s="203" t="str">
         <f t="shared" ref="L22" si="123">MID(TEXT(HEX2BIN($I21,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
-      <c r="M22" s="205" t="str">
+      <c r="M22" s="204" t="str">
         <f t="shared" ref="M22" si="124">MID(TEXT(HEX2BIN($M21,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="N22" s="206" t="str">
+      <c r="N22" s="205" t="str">
         <f t="shared" ref="N22" si="125">MID(TEXT(HEX2BIN($M21,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="O22" s="206" t="str">
+      <c r="O22" s="205" t="str">
         <f t="shared" ref="O22" si="126">MID(TEXT(HEX2BIN($M21,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="P22" s="207" t="str">
+      <c r="P22" s="206" t="str">
         <f t="shared" ref="P22" si="127">MID(TEXT(HEX2BIN($M21,4),"0000"),4,1)</f>
         <v>1</v>
       </c>
-      <c r="Q22" s="208" t="str">
+      <c r="Q22" s="207" t="str">
         <f t="shared" ref="Q22" si="128">MID(TEXT(HEX2BIN($Q21,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="R22" s="209" t="str">
+      <c r="R22" s="208" t="str">
         <f t="shared" ref="R22" si="129">MID(TEXT(HEX2BIN($Q21,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="S22" s="209" t="str">
+      <c r="S22" s="208" t="str">
         <f t="shared" ref="S22" si="130">MID(TEXT(HEX2BIN($Q21,4),"0000"),3,1)</f>
         <v>1</v>
       </c>
-      <c r="T22" s="209" t="str">
+      <c r="T22" s="208" t="str">
         <f t="shared" ref="T22" si="131">MID(TEXT(HEX2BIN($Q21,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="U22" s="210" t="str">
+      <c r="U22" s="209" t="str">
         <f t="shared" ref="U22" si="132">MID(TEXT(HEX2BIN($U21,4),"0000"),1,1)</f>
         <v>0</v>
       </c>
-      <c r="V22" s="209" t="str">
+      <c r="V22" s="208" t="str">
         <f t="shared" ref="V22" si="133">MID(TEXT(HEX2BIN($U21,4),"0000"),2,1)</f>
         <v>0</v>
       </c>
-      <c r="W22" s="209" t="str">
+      <c r="W22" s="208" t="str">
         <f t="shared" ref="W22" si="134">MID(TEXT(HEX2BIN($U21,4),"0000"),3,1)</f>
         <v>0</v>
       </c>
-      <c r="X22" s="211" t="str">
+      <c r="X22" s="210" t="str">
         <f t="shared" ref="X22" si="135">MID(TEXT(HEX2BIN($U21,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
@@ -20523,7 +20559,7 @@
       <c r="C23" s="186"/>
       <c r="D23" s="187"/>
       <c r="E23" s="186" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F23" s="186"/>
       <c r="G23" s="186"/>
@@ -20547,7 +20583,7 @@
       <c r="S23" s="186"/>
       <c r="T23" s="186"/>
       <c r="U23" s="188" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="V23" s="186"/>
       <c r="W23" s="186"/>
@@ -20570,19 +20606,19 @@
         <f t="shared" ref="D24" si="139">MID(TEXT(HEX2BIN($A23,4),"0000"),4,1)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="198" t="str">
+      <c r="E24" s="197" t="str">
         <f t="shared" ref="E24" si="140">MID(TEXT(HEX2BIN($E23,4),"0000"),1,1)</f>
         <v>1</v>
       </c>
-      <c r="F24" s="198" t="str">
+      <c r="F24" s="197" t="str">
         <f t="shared" ref="F24" si="141">MID(TEXT(HEX2BIN($E23,4),"0000"),2,1)</f>
         <v>1</v>
       </c>
-      <c r="G24" s="198" t="str">
+      <c r="G24" s="197" t="str">
         <f t="shared" ref="G24" si="142">MID(TEXT(HEX2BIN($E23,4),"0000"),3,1)</f>
         <v>1</v>
       </c>
-      <c r="H24" s="199" t="str">
+      <c r="H24" s="198" t="str">
         <f t="shared" ref="H24" si="143">MID(TEXT(HEX2BIN($E23,4),"0000"),4,1)</f>
         <v>0</v>
       </c>

</xml_diff>